<commit_message>
Added functionality to pull multiple modules at once for avg prod tt and bin 98/99 Prints output of bin98/99 and TT to csv files
</commit_message>
<xml_diff>
--- a/OpenIssuesTracker.xlsx
+++ b/OpenIssuesTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/aoife_barnes_intel_com/Documents/Scripts/Array Mail/Array_Summary_GUI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{967C14AD-E0E2-4F83-B6C3-E196E7601CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5E28496-3821-41D2-9763-73084F88F65D}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{967C14AD-E0E2-4F83-B6C3-E196E7601CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71554A16-6D01-420D-A63D-A870A632B6B7}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-75" windowWidth="38640" windowHeight="21120" xr2:uid="{5025D52B-E805-4380-9A7A-BBB380D6B08F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5025D52B-E805-4380-9A7A-BBB380D6B08F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Owner</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Print results to text file output as well as email?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can we add the total number of dies/wafer pulled here for B98/99 data in the email? </t>
+  </si>
+  <si>
+    <t>23WW05.1</t>
   </si>
 </sst>
 </file>
@@ -312,8 +318,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -332,13 +345,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Accent4" xfId="1" builtinId="43"/>
@@ -368,6 +376,50 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -416,58 +468,6 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -501,6 +501,44 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -534,36 +572,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -578,20 +586,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE5117ED-20EC-417D-BC86-A81A131901DA}" name="Table1" displayName="Table1" ref="A3:F10" totalsRowShown="0" headerRowDxfId="9" dataDxfId="6" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
-  <autoFilter ref="A3:F10" xr:uid="{EE5117ED-20EC-417D-BC86-A81A131901DA}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:F10">
-    <sortCondition descending="1" ref="D3:D10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE5117ED-20EC-417D-BC86-A81A131901DA}" name="Table1" displayName="Table1" ref="A3:F11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A3:F11" xr:uid="{EE5117ED-20EC-417D-BC86-A81A131901DA}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:F11">
+    <sortCondition descending="1" ref="D3:D11"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{24C983E2-3DEC-4F22-A799-6A9D11046F1D}" name="Owner" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{17B7ACA5-D5A1-4F53-84E6-054D7DA35A83}" name="Product Code" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{24C983E2-3DEC-4F22-A799-6A9D11046F1D}" name="Owner" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{17B7ACA5-D5A1-4F53-84E6-054D7DA35A83}" name="Product Code" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{5C9C37BD-FEFF-4FEA-B096-AC936EAC6A3B}" name="Issued Identified" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{1E88F98A-6D3F-4F41-AADA-CFC434290E69}" name="Status" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{1E88F98A-6D3F-4F41-AADA-CFC434290E69}" name="Status" dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{75E44CD8-7078-4540-8727-ECAF39C53D37}" name="Resolution Date" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{E1F530EF-9398-46C8-BB02-ACD77C343ECA}" name="Resolution Git Commit" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{75E44CD8-7078-4540-8727-ECAF39C53D37}" name="Resolution Date" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{E1F530EF-9398-46C8-BB02-ACD77C343ECA}" name="Resolution Git Commit" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -894,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E233D192-C9B7-4D09-BAD9-A76AF8C6B7B2}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -911,164 +919,187 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="15" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
         <v>Open</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
-        <v>Open</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+        <v>N/A</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
-        <v>Open</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+        <v>N/A</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="str">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
         <v>N/A</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="str">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
-        <v>N/A</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+        <v>Closed</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="str">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
-        <v>N/A</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
+        <v>Closed</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="10" t="str">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="4" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
         <v>Closed</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
+        <v>Closed</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F11" s="4" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <protectedRanges>
-    <protectedRange algorithmName="SHA-512" hashValue="pR1ejdyl/zb/sLjjdzUb4Ln2iwYVWxjh7PjzdcVbsOIJDyNqOHqXbsW3a5KadWThEYLw4daUo4BzAZxSrUWA8Q==" saltValue="QoWAq6PjOGRKGLw1cj6AQQ==" spinCount="100000" sqref="D3:F10" name="Range1"/>
+    <protectedRange algorithmName="SHA-512" hashValue="pR1ejdyl/zb/sLjjdzUb4Ln2iwYVWxjh7PjzdcVbsOIJDyNqOHqXbsW3a5KadWThEYLw4daUo4BzAZxSrUWA8Q==" saltValue="QoWAq6PjOGRKGLw1cj6AQQ==" spinCount="100000" sqref="D3:F11" name="Range1"/>
   </protectedRanges>
   <mergeCells count="1">
     <mergeCell ref="A1:F2"/>

</xml_diff>

<commit_message>
Vmin plots & repeatability
</commit_message>
<xml_diff>
--- a/OpenIssuesTracker.xlsx
+++ b/OpenIssuesTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/aoife_barnes_intel_com/Documents/Scripts/Array Mail/Array_Summary_GUI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{967C14AD-E0E2-4F83-B6C3-E196E7601CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71554A16-6D01-420D-A63D-A870A632B6B7}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{967C14AD-E0E2-4F83-B6C3-E196E7601CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7CE957B-C363-478B-B7D6-77CAE1AD497F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5025D52B-E805-4380-9A7A-BBB380D6B08F}"/>
+    <workbookView visibility="hidden" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5025D52B-E805-4380-9A7A-BBB380D6B08F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Owner</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>23WW05.1</t>
+  </si>
+  <si>
+    <t>Barnes, Aoife</t>
+  </si>
+  <si>
+    <t>Vmin plots (for optimsation) - WIP just need to get JMPbackgroundcaller working.</t>
+  </si>
+  <si>
+    <t>Vmin repeatability plots</t>
   </si>
 </sst>
 </file>
@@ -318,7 +327,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -327,6 +336,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -345,8 +359,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Accent4" xfId="1" builtinId="43"/>
@@ -586,10 +598,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE5117ED-20EC-417D-BC86-A81A131901DA}" name="Table1" displayName="Table1" ref="A3:F11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="A3:F11" xr:uid="{EE5117ED-20EC-417D-BC86-A81A131901DA}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:F11">
-    <sortCondition descending="1" ref="D3:D11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE5117ED-20EC-417D-BC86-A81A131901DA}" name="Table1" displayName="Table1" ref="A3:F13" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A3:F13" xr:uid="{EE5117ED-20EC-417D-BC86-A81A131901DA}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:F13">
+    <sortCondition descending="1" ref="D3:D13"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{24C983E2-3DEC-4F22-A799-6A9D11046F1D}" name="Owner" dataDxfId="7"/>
@@ -902,41 +914,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E233D192-C9B7-4D09-BAD9-A76AF8C6B7B2}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A7" sqref="A7:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="79.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -956,59 +968,59 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="15" t="str">
+      <c r="D4" s="9" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
         <v>Open</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="9" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
+        <v>Open</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="9" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
+        <v>Open</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
-        <v>N/A</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
-        <v>N/A</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="str">
@@ -1018,45 +1030,37 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>19</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="4" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
-        <v>Closed</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>N/A</v>
+      </c>
+      <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C9" s="4"/>
       <c r="D9" s="4" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
-        <v>Closed</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>N/A</v>
+      </c>
+      <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1064,7 +1068,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="4" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
@@ -1073,33 +1077,77 @@
       <c r="E10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>10</v>
+      <c r="F10" s="10">
+        <v>3102280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D11" s="4" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
         <v>Closed</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="10">
+        <v>3102280</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="4" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
+        <v>Closed</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="10">
+        <v>3102280</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="4" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[Issued Identified]]), "N/A", IF(AND(ISBLANK(Table1[[#This Row],[Resolution Date]]),ISBLANK(Table1[[#This Row],[Resolution Git Commit]])), "Open", "Closed"))</f>
+        <v>Closed</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <protectedRanges>
-    <protectedRange algorithmName="SHA-512" hashValue="pR1ejdyl/zb/sLjjdzUb4Ln2iwYVWxjh7PjzdcVbsOIJDyNqOHqXbsW3a5KadWThEYLw4daUo4BzAZxSrUWA8Q==" saltValue="QoWAq6PjOGRKGLw1cj6AQQ==" spinCount="100000" sqref="D3:F11" name="Range1"/>
+    <protectedRange algorithmName="SHA-512" hashValue="pR1ejdyl/zb/sLjjdzUb4Ln2iwYVWxjh7PjzdcVbsOIJDyNqOHqXbsW3a5KadWThEYLw4daUo4BzAZxSrUWA8Q==" saltValue="QoWAq6PjOGRKGLw1cj6AQQ==" spinCount="100000" sqref="D3:F13" name="Range1"/>
   </protectedRanges>
   <mergeCells count="1">
     <mergeCell ref="A1:F2"/>
@@ -1112,10 +1160,15 @@
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="F10" r:id="rId1" display="https://github.com/aoifebar/Array-Summary-GUI/commit/3102280cb84dce10fa6400af0d338253873d60cd" xr:uid="{FB3AB110-B491-405A-ABB2-B61FCAAE66FD}"/>
+    <hyperlink ref="F11" r:id="rId2" display="https://github.com/aoifebar/Array-Summary-GUI/commit/3102280cb84dce10fa6400af0d338253873d60cd" xr:uid="{6A2C98D7-A8C2-41F7-8C3C-608FBE1CF49C}"/>
+    <hyperlink ref="F12" r:id="rId3" display="https://github.com/aoifebar/Array-Summary-GUI/commit/3102280cb84dce10fa6400af0d338253873d60cd" xr:uid="{5BB401CE-1B56-4535-B5DC-FCDDC89F263F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>